<commit_message>
Update AR in Education SLR (Responses)_all2023.xlsx
</commit_message>
<xml_diff>
--- a/data/update_2023/AR in Education SLR (Responses)_all2023.xlsx
+++ b/data/update_2023/AR in Education SLR (Responses)_all2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smasneri\CODE\AR_SLR_Paper\data\update_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4D6855-1FFD-4FDB-A649-183A1F78A937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAF32C9-157D-4A92-A4D7-570B93F60F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="20010" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="Subjects" localSheetId="1">OnlyValid!$I$2:$I$80</definedName>
     <definedName name="Subjects">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31688,14 +31688,17 @@
   <dimension ref="A1:BE602"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O136" sqref="O136"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D116" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="L102" sqref="L102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.28515625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="84" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="57" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="57" customWidth="1"/>

</xml_diff>